<commit_message>
Data Preprocessing notes loaded
</commit_message>
<xml_diff>
--- a/ML_AZ_Resources/ML_Notes.xlsx
+++ b/ML_AZ_Resources/ML_Notes.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="135">
   <si>
     <t>overview of ML starts</t>
   </si>
@@ -132,6 +132,303 @@
   </si>
   <si>
     <t>Normalization</t>
+  </si>
+  <si>
+    <t>10.3.2</t>
+  </si>
+  <si>
+    <t>All values will be between 0 and 1</t>
+  </si>
+  <si>
+    <t>Standardization</t>
+  </si>
+  <si>
+    <t>All values will be between -3 and 3</t>
+  </si>
+  <si>
+    <t>Example of Standardization and Normalization</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Salary</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>After Standardization</t>
+  </si>
+  <si>
+    <t>Feature Scaling ends</t>
+  </si>
+  <si>
+    <t>Steps</t>
+  </si>
+  <si>
+    <t>import libraries</t>
+  </si>
+  <si>
+    <t>import data set</t>
+  </si>
+  <si>
+    <t>take care of missing data</t>
+  </si>
+  <si>
+    <t>encoding categorical data</t>
+  </si>
+  <si>
+    <t>encoding independent variables</t>
+  </si>
+  <si>
+    <t>encoding dependent variables</t>
+  </si>
+  <si>
+    <t>spliting dataset into training and test sets</t>
+  </si>
+  <si>
+    <t>apply feature scaling</t>
+  </si>
+  <si>
+    <t>12.4.1</t>
+  </si>
+  <si>
+    <t>12.4.2</t>
+  </si>
+  <si>
+    <t>Example with code</t>
+  </si>
+  <si>
+    <t># import dataset.</t>
+  </si>
+  <si>
+    <t># .values converts the dataframe into list of lists</t>
+  </si>
+  <si>
+    <t>import numpy as np</t>
+  </si>
+  <si>
+    <t>import matplotlib.pyplot as plt</t>
+  </si>
+  <si>
+    <t>import pandas as pd</t>
+  </si>
+  <si>
+    <t>dataset = pd.read_csv("data\\Data.csv")</t>
+  </si>
+  <si>
+    <t>X = dataset.iloc[:,:-1].values</t>
+  </si>
+  <si>
+    <t>Y = dataset.iloc[:,-1].values</t>
+  </si>
+  <si>
+    <t>print(X)</t>
+  </si>
+  <si>
+    <t>print("--")</t>
+  </si>
+  <si>
+    <t>imputer = SimpleImputer(missing_values=np.nan, strategy='mean')</t>
+  </si>
+  <si>
+    <t>X[:,1:3] = imputer.transform(X[:,1:3])</t>
+  </si>
+  <si>
+    <t xml:space="preserve">from sklearn.impute import SimpleImputer  </t>
+  </si>
+  <si>
+    <t># SimpleImputer imported</t>
+  </si>
+  <si>
+    <t xml:space="preserve">imputer.fit(X[:,1:3]) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> #X is a list, converted by using .values from dataframe. 1:3 means leave 0th and 3rd column as only numeric columns should be considered</t>
+  </si>
+  <si>
+    <t># this will print list X with no nan</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Purchased</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Spain</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Featuer</t>
+  </si>
+  <si>
+    <t>dependent Variable</t>
+  </si>
+  <si>
+    <t>features are columns used for prediction</t>
+  </si>
+  <si>
+    <t>To take all columns except last .iloc[:,-1] was used</t>
+  </si>
+  <si>
+    <t>OneHotEncoder: Often there are text featues which are difficult to use in modeling and hence these need to be converted into numeric codes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">these codes do not have any weight or preference meaning. For example if we have 3 countries (germany, france,  spane) ,we can have [1 0 0] [0 1 0] and [0 0 1] </t>
+  </si>
+  <si>
+    <t>yes and no can be replaced by 1 and 0</t>
+  </si>
+  <si>
+    <t># OneHoteEncoder converts a category into code like [0 1 0] etc.</t>
+  </si>
+  <si>
+    <t># here two classes are used... ColumnTransformer and OneHotEncoder</t>
+  </si>
+  <si>
+    <t># the 'transformers' argument takes parameters in form of a list</t>
+  </si>
+  <si>
+    <t># transformers=[('encoder', OneHotEncoder(),[0])] tells what type of transformation is needed</t>
+  </si>
+  <si>
+    <t># the [0] tells that the transformation is to be applied on 0th column</t>
+  </si>
+  <si>
+    <t># remainder='passthrough' tells that the other columns should remain as they are and not dropped</t>
+  </si>
+  <si>
+    <t># np.array is called to force the output as array</t>
+  </si>
+  <si>
+    <t># fit_transform .. here this method does both fit and trasform in one step</t>
+  </si>
+  <si>
+    <t>X = np.array(ct.fit_transform(X))</t>
+  </si>
+  <si>
+    <t>from sklearn.compose import ColumnTransformer</t>
+  </si>
+  <si>
+    <t>from sklearn.preprocessing import OneHotEncoder</t>
+  </si>
+  <si>
+    <t>ct = ColumnTransformer( transformers=[('encoder', OneHotEncoder(),[0])], remainder='passthrough')</t>
+  </si>
+  <si>
+    <t>from sklearn.preprocessing import LabelEncoder</t>
+  </si>
+  <si>
+    <t>le = LabelEncoder()</t>
+  </si>
+  <si>
+    <t>Y = le.fit_transform(Y)</t>
+  </si>
+  <si>
+    <t>print(Y)</t>
+  </si>
+  <si>
+    <t># now yes and no can be converted into 1 and 0</t>
+  </si>
+  <si>
+    <t>Feature scaling should be applied AFTER data is slit</t>
+  </si>
+  <si>
+    <t>Split data in train and test sets</t>
+  </si>
+  <si>
+    <t>sklearn has module that can be used to split the data… 4 sets (X_Train, X_test, Y_Train, Y_Test) will be obtained</t>
+  </si>
+  <si>
+    <t>#Above code does not have the feature scaling</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> so it is ok. to split.</t>
+  </si>
+  <si>
+    <t>from sklearn.model_selection import  train_test_split</t>
+  </si>
+  <si>
+    <t>X_train, X_test, Y_train, Y_test = train_test_split(X,Y, test_size= 0.2, random_state=1)</t>
+  </si>
+  <si>
+    <t>Split</t>
+  </si>
+  <si>
+    <t>Feature scaling on data that is already splitted</t>
+  </si>
+  <si>
+    <t>Feature scaling is not applied in all models. For example in multiple regression, as each variable (x1,x2,x3..) is multiplied by a coefficent(b1,b2,b3…) . The coefficients will take smaller values while learning</t>
+  </si>
+  <si>
+    <t>Works in ALL situations</t>
+  </si>
+  <si>
+    <t>Use only when data is Normall distributed in ALL THE FEATURES</t>
+  </si>
+  <si>
+    <t>from sklearn.preprocessing import StandardScaler</t>
+  </si>
+  <si>
+    <t>#instance of StandardScaler is created</t>
+  </si>
+  <si>
+    <t>sc = StandardScaler()</t>
+  </si>
+  <si>
+    <t># here fit_transform is used as it will fit sc object and find mean</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SD etc</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> then transform in one step</t>
+  </si>
+  <si>
+    <t>X_train[:</t>
+  </si>
+  <si>
+    <t>3:] = sc.fit_transform(X_train[:</t>
+  </si>
+  <si>
+    <t>3:])</t>
+  </si>
+  <si>
+    <t># for test test</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the fit is not applied as it has to use the same statistical values from training for test</t>
+  </si>
+  <si>
+    <t>X_test[:</t>
+  </si>
+  <si>
+    <t>3:] = sc.transform(X_test[:</t>
+  </si>
+  <si>
+    <t>print(X_train)</t>
+  </si>
+  <si>
+    <t>print(X_test)</t>
   </si>
 </sst>
 </file>
@@ -147,17 +444,53 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -167,8 +500,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -184,6 +521,176 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>388354</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3114675" y="4886324"/>
+          <a:ext cx="2150479" cy="1095375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3400425" y="6524625"/>
+          <a:ext cx="1371600" cy="685800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>151628</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7991475" y="7581128"/>
+          <a:ext cx="3028950" cy="1181872"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -449,13 +956,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:Q126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="A128" sqref="A128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="15" max="15" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1">
@@ -577,7 +1087,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>9.1</v>
       </c>
@@ -585,7 +1095,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>9.1999999999999993</v>
       </c>
@@ -593,7 +1103,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>9.3000000000000007</v>
       </c>
@@ -601,12 +1111,15 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>9</v>
+      </c>
       <c r="B20" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>10</v>
       </c>
@@ -614,7 +1127,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>10.1</v>
       </c>
@@ -622,7 +1135,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>10.199999999999999</v>
       </c>
@@ -630,7 +1143,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>10.3</v>
       </c>
@@ -638,7 +1151,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>34</v>
       </c>
@@ -646,7 +1159,630 @@
         <v>35</v>
       </c>
     </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J28" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J29" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>36</v>
+      </c>
+      <c r="D35" t="s">
+        <v>38</v>
+      </c>
+      <c r="J35" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J36" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>10.4</v>
+      </c>
+      <c r="C40" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K41" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D42" s="1"/>
+      <c r="E42" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J42" s="1"/>
+      <c r="K42" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L42" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D43" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E43" s="1">
+        <v>70000</v>
+      </c>
+      <c r="F43" s="1">
+        <v>45</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K43" s="1">
+        <f>(E43-E45)/(E43-E45)</f>
+        <v>1</v>
+      </c>
+      <c r="L43" s="1">
+        <f>(F43-F45)/(F43-F45)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D44" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E44" s="1">
+        <v>60000</v>
+      </c>
+      <c r="F44" s="1">
+        <v>44</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K44" s="1">
+        <f>(E44-E45)/(E43-E45)</f>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="L44" s="1">
+        <f>(F44-F45)/(F43-F45)</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D45" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E45" s="1">
+        <v>52000</v>
+      </c>
+      <c r="F45" s="1">
+        <v>40</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K45" s="1">
+        <f>(E45-E45)/(E43-E45)</f>
+        <v>0</v>
+      </c>
+      <c r="L45" s="1">
+        <f>(F45-F45)/(F43-F45)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>10</v>
+      </c>
+      <c r="B46" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>12</v>
+      </c>
+      <c r="B48" t="s">
+        <v>48</v>
+      </c>
+      <c r="L48" t="s">
+        <v>84</v>
+      </c>
+      <c r="M48" t="s">
+        <v>84</v>
+      </c>
+      <c r="N48" t="s">
+        <v>84</v>
+      </c>
+      <c r="O48" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B49">
+        <v>12.1</v>
+      </c>
+      <c r="C49" t="s">
+        <v>49</v>
+      </c>
+      <c r="L49" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="M49" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="N49" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="O49" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q49" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B50">
+        <v>12.2</v>
+      </c>
+      <c r="C50" t="s">
+        <v>50</v>
+      </c>
+      <c r="L50" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="M50" s="2">
+        <v>44</v>
+      </c>
+      <c r="N50" s="2">
+        <v>72000</v>
+      </c>
+      <c r="O50" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B51">
+        <v>12.3</v>
+      </c>
+      <c r="C51" t="s">
+        <v>51</v>
+      </c>
+      <c r="L51" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="M51" s="2">
+        <v>27</v>
+      </c>
+      <c r="N51" s="2">
+        <v>48000</v>
+      </c>
+      <c r="O51" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B52">
+        <v>12.4</v>
+      </c>
+      <c r="C52" t="s">
+        <v>52</v>
+      </c>
+      <c r="L52" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="M52" s="2">
+        <v>30</v>
+      </c>
+      <c r="N52" s="2">
+        <v>54000</v>
+      </c>
+      <c r="O52" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>57</v>
+      </c>
+      <c r="D53" t="s">
+        <v>53</v>
+      </c>
+      <c r="L53" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="M53" s="2">
+        <v>38</v>
+      </c>
+      <c r="N53" s="2">
+        <v>61000</v>
+      </c>
+      <c r="O53" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>58</v>
+      </c>
+      <c r="D54" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B55">
+        <v>12.5</v>
+      </c>
+      <c r="C55" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B56">
+        <v>12.6</v>
+      </c>
+      <c r="C56" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>13</v>
+      </c>
+      <c r="B58" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B59">
+        <v>13.1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C61" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C62" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C64" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="65" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C65" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="66" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C66" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C67" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C68" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C69" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C70" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C71" t="s">
+        <v>72</v>
+      </c>
+      <c r="J71" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="72" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C72" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="73" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C73" t="s">
+        <v>74</v>
+      </c>
+      <c r="J73" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="74" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C74" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="75" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C75" t="s">
+        <v>68</v>
+      </c>
+      <c r="G75" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="80" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B80">
+        <v>13.2</v>
+      </c>
+      <c r="C80" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="81" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C81" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="82" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C82" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="84" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C84" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="85" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C85" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="86" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C86" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="88" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C88" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="89" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C89" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="90" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C90" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="91" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C91" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="92" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C92" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="93" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C93" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="94" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C94" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="96" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C96" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C97" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C98" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C100" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C101" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C102" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C103" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C104" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>23</v>
+      </c>
+      <c r="B107" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B108">
+        <v>23.1</v>
+      </c>
+      <c r="C108" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B109">
+        <v>23.2</v>
+      </c>
+      <c r="C109" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B110">
+        <v>23.3</v>
+      </c>
+      <c r="C110" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C111" t="s">
+        <v>111</v>
+      </c>
+      <c r="D111" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C112" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C113" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>24</v>
+      </c>
+      <c r="B115" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B116">
+        <v>24.1</v>
+      </c>
+      <c r="C116" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C117" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C118" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C119" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C120" t="s">
+        <v>123</v>
+      </c>
+      <c r="D120" t="s">
+        <v>124</v>
+      </c>
+      <c r="E120" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C121" t="s">
+        <v>126</v>
+      </c>
+      <c r="D121" t="s">
+        <v>127</v>
+      </c>
+      <c r="E121" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C122" t="s">
+        <v>129</v>
+      </c>
+      <c r="D122" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C123" t="s">
+        <v>131</v>
+      </c>
+      <c r="D123" t="s">
+        <v>132</v>
+      </c>
+      <c r="E123" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C124" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C125" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C126" t="s">
+        <v>134</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Baisc steps completed to start with regression and other modules
</commit_message>
<xml_diff>
--- a/ML_AZ_Resources/ML_Notes.xlsx
+++ b/ML_AZ_Resources/ML_Notes.xlsx
@@ -12,7 +12,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="7620"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Basic Steps" sheetId="1" r:id="rId1"/>
+    <sheet name="All_RegressionModels" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="193">
   <si>
     <t>overview of ML starts</t>
   </si>
@@ -429,6 +430,180 @@
   </si>
   <si>
     <t>print(X_test)</t>
+  </si>
+  <si>
+    <t>Simple Linear Regression</t>
+  </si>
+  <si>
+    <t># Splitting the dataset into the Training set and Test set</t>
+  </si>
+  <si>
+    <t>from sklearn.model_selection import train_test_split</t>
+  </si>
+  <si>
+    <t>X_train, X_test, y_train, y_test = train_test_split(X, y, test_size = 1/3, random_state = 0)</t>
+  </si>
+  <si>
+    <t># Training the Simple Linear Regression model on the Training set</t>
+  </si>
+  <si>
+    <t>from sklearn.linear_model import LinearRegression</t>
+  </si>
+  <si>
+    <t>regressor = LinearRegression()</t>
+  </si>
+  <si>
+    <t>regressor.fit(X_train, y_train)</t>
+  </si>
+  <si>
+    <t># Predicting the Test set results</t>
+  </si>
+  <si>
+    <t>y_pred = regressor.predict(X_test)</t>
+  </si>
+  <si>
+    <t># Visualising the Training set results</t>
+  </si>
+  <si>
+    <t>plt.scatter(X_train, y_train, color = 'red')</t>
+  </si>
+  <si>
+    <t>plt.plot(X_train, regressor.predict(X_train), color = 'blue')</t>
+  </si>
+  <si>
+    <t>plt.title('Salary vs Experience (Training set)')</t>
+  </si>
+  <si>
+    <t>plt.xlabel('Years of Experience')</t>
+  </si>
+  <si>
+    <t>plt.ylabel('Salary')</t>
+  </si>
+  <si>
+    <t>plt.show()</t>
+  </si>
+  <si>
+    <t># Visualising the Test set results</t>
+  </si>
+  <si>
+    <t>plt.scatter(X_test, y_test, color = 'red')</t>
+  </si>
+  <si>
+    <t>plt.title('Salary vs Experience (Test set)')</t>
+  </si>
+  <si>
+    <t>Dealing with Missing data</t>
+  </si>
+  <si>
+    <t>#here .values is used so that the output is an array. This will facilitate the later processes where list is needed</t>
+  </si>
+  <si>
+    <t>13.0.1</t>
+  </si>
+  <si>
+    <t>modules needed</t>
+  </si>
+  <si>
+    <t>13.0.1.1</t>
+  </si>
+  <si>
+    <t>from sklearn.impute import SimpleImputer</t>
+  </si>
+  <si>
+    <t>Missing Data</t>
+  </si>
+  <si>
+    <t>13.0.1.1.1</t>
+  </si>
+  <si>
+    <t>13.0.1.2</t>
+  </si>
+  <si>
+    <t>imputer.fit(X[:,1:])</t>
+  </si>
+  <si>
+    <t>X[:,1:] = imputer.transform(X[:,1:])</t>
+  </si>
+  <si>
+    <t>13.0.1.1.2</t>
+  </si>
+  <si>
+    <t>13.0.1.1.3</t>
+  </si>
+  <si>
+    <t>13.0.1.1.4</t>
+  </si>
+  <si>
+    <t>Encoding Categorical data</t>
+  </si>
+  <si>
+    <t>13.0.1.2.1</t>
+  </si>
+  <si>
+    <t>from sklearn.preprocessing import OneHotEncoder, LabelEncoder</t>
+  </si>
+  <si>
+    <t>ct = ColumnTransformer(transformers=[('encoder', OneHotEncoder(), [0])], remainder='passthrough')</t>
+  </si>
+  <si>
+    <t>X = np.array( ct.fit_transform(X))</t>
+  </si>
+  <si>
+    <t>13.0.1.2.2</t>
+  </si>
+  <si>
+    <t>13.0.1.2.3</t>
+  </si>
+  <si>
+    <t>13.0.1.2.4</t>
+  </si>
+  <si>
+    <t>le.fit_transform(Y)</t>
+  </si>
+  <si>
+    <t>13.0.1.2.5</t>
+  </si>
+  <si>
+    <t>13.0.1.2.6</t>
+  </si>
+  <si>
+    <t>13.0.1.3</t>
+  </si>
+  <si>
+    <t>Test Train Split</t>
+  </si>
+  <si>
+    <t>13.0.1.3.1</t>
+  </si>
+  <si>
+    <t>13.0.1.3.2</t>
+  </si>
+  <si>
+    <t>X_Train, X_Test, Y_Train, Y_Test = train_test_split(X,Y, test_size=.2, random_state=1)</t>
+  </si>
+  <si>
+    <t>13.0.1.4</t>
+  </si>
+  <si>
+    <t>Feature Scaling</t>
+  </si>
+  <si>
+    <t>13.0.1.4.1</t>
+  </si>
+  <si>
+    <t>X_Train[:,3:] = sc.fit_transform(X_Train[:,3:])</t>
+  </si>
+  <si>
+    <t>X_Test[:,3:] = sc.transform(X_Test[:,3:])</t>
+  </si>
+  <si>
+    <t>13.0.1.4.2</t>
+  </si>
+  <si>
+    <t>13.0.1.4.3</t>
+  </si>
+  <si>
+    <t>13.0.1.4.4</t>
   </si>
 </sst>
 </file>
@@ -956,10 +1131,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q126"/>
+  <dimension ref="A1:Q147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="A128" sqref="A128"/>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="K88" sqref="K88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1438,345 +1613,519 @@
         <v>56</v>
       </c>
     </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>13</v>
+      </c>
+      <c r="B57" t="s">
+        <v>59</v>
+      </c>
+    </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>13</v>
-      </c>
       <c r="B58" t="s">
-        <v>59</v>
+        <v>157</v>
+      </c>
+      <c r="C58" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B59">
-        <v>13.1</v>
+      <c r="C59" t="s">
+        <v>159</v>
+      </c>
+      <c r="D59" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C60" t="s">
-        <v>62</v>
+      <c r="D60" t="s">
+        <v>162</v>
+      </c>
+      <c r="E60" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C61" t="s">
-        <v>63</v>
+      <c r="D61" t="s">
+        <v>166</v>
+      </c>
+      <c r="E61" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C62" t="s">
-        <v>64</v>
+      <c r="D62" t="s">
+        <v>167</v>
+      </c>
+      <c r="E62" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D63" t="s">
+        <v>168</v>
+      </c>
+      <c r="E63" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C64" t="s">
+        <v>163</v>
+      </c>
+      <c r="D64" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D65" t="s">
+        <v>170</v>
+      </c>
+      <c r="E65" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D66" t="s">
+        <v>174</v>
+      </c>
+      <c r="E66" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D67" t="s">
+        <v>175</v>
+      </c>
+      <c r="E67" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D68" t="s">
+        <v>176</v>
+      </c>
+      <c r="E68" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D69" t="s">
+        <v>178</v>
+      </c>
+      <c r="E69" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D70" t="s">
+        <v>179</v>
+      </c>
+      <c r="E70" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C71" t="s">
+        <v>180</v>
+      </c>
+      <c r="D71" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D72" t="s">
+        <v>182</v>
+      </c>
+      <c r="E72" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D73" t="s">
+        <v>183</v>
+      </c>
+      <c r="E73" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="74" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C74" t="s">
+        <v>185</v>
+      </c>
+      <c r="D74" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="75" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D75" t="s">
+        <v>187</v>
+      </c>
+      <c r="E75" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="76" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D76" t="s">
+        <v>190</v>
+      </c>
+      <c r="E76" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="77" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D77" t="s">
+        <v>191</v>
+      </c>
+      <c r="E77" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="78" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D78" t="s">
+        <v>192</v>
+      </c>
+      <c r="E78" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="80" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B80">
+        <v>13.1</v>
+      </c>
+      <c r="C80" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="81" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C81" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="82" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C82" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="83" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C83" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="85" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C85" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="65" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C65" t="s">
+    <row r="86" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C86" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="66" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C66" t="s">
+    <row r="87" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C87" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C67" t="s">
+    <row r="88" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C88" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="68" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C68" t="s">
+      <c r="J88" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="89" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C89" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C69" t="s">
+    <row r="90" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C90" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C70" t="s">
+    <row r="91" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C91" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C71" t="s">
+    <row r="92" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C92" t="s">
         <v>72</v>
       </c>
-      <c r="J71" t="s">
+      <c r="J92" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="72" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C72" t="s">
+    <row r="93" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C93" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C73" t="s">
+    <row r="94" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C94" t="s">
         <v>74</v>
       </c>
-      <c r="J73" t="s">
+      <c r="J94" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="74" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C74" t="s">
+    <row r="95" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C95" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="75" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C75" t="s">
+    <row r="96" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C96" t="s">
         <v>68</v>
       </c>
-      <c r="G75" t="s">
+      <c r="G96" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="80" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B80">
+    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B101">
         <v>13.2</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C101" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="81" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C81" t="s">
+    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C102" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="82" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C82" t="s">
+    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C103" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="84" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C84" t="s">
+    <row r="105" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C105" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="85" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C85" t="s">
+    <row r="106" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C106" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="86" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C86" t="s">
+    <row r="107" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C107" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="88" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C88" t="s">
+    <row r="109" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C109" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="89" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C89" t="s">
+    <row r="110" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C110" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="90" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C90" t="s">
+    <row r="111" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C111" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="91" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C91" t="s">
+    <row r="112" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C112" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="92" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C92" t="s">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C113" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="93" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C93" t="s">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C114" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="94" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C94" t="s">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C115" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="96" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C96" t="s">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C117" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C97" t="s">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C118" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C98" t="s">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C119" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C100" t="s">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C121" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C101" t="s">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C122" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C102" t="s">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C123" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C103" t="s">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C124" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C104" t="s">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C125" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128">
         <v>23</v>
       </c>
-      <c r="B107" t="s">
+      <c r="B128" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B108">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B129">
         <v>23.1</v>
       </c>
-      <c r="C108" t="s">
+      <c r="C129" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B109">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B130">
         <v>23.2</v>
       </c>
-      <c r="C109" t="s">
+      <c r="C130" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B110">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B131">
         <v>23.3</v>
       </c>
-      <c r="C110" t="s">
+      <c r="C131" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C111" t="s">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C132" t="s">
         <v>111</v>
       </c>
-      <c r="D111" t="s">
+      <c r="D132" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C112" t="s">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C133" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C113" t="s">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C134" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A115">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136">
         <v>24</v>
       </c>
-      <c r="B115" t="s">
+      <c r="B136" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B116">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B137">
         <v>24.1</v>
       </c>
-      <c r="C116" t="s">
+      <c r="C137" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C117" t="s">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C138" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C118" t="s">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C139" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C119" t="s">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C140" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C120" t="s">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C141" t="s">
         <v>123</v>
       </c>
-      <c r="D120" t="s">
+      <c r="D141" t="s">
         <v>124</v>
       </c>
-      <c r="E120" t="s">
+      <c r="E141" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C121" t="s">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C142" t="s">
         <v>126</v>
       </c>
-      <c r="D121" t="s">
+      <c r="D142" t="s">
         <v>127</v>
       </c>
-      <c r="E121" t="s">
+      <c r="E142" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C122" t="s">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C143" t="s">
         <v>129</v>
       </c>
-      <c r="D122" t="s">
+      <c r="D143" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C123" t="s">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C144" t="s">
         <v>131</v>
       </c>
-      <c r="D123" t="s">
+      <c r="D144" t="s">
         <v>132</v>
       </c>
-      <c r="E123" t="s">
+      <c r="E144" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C124" t="s">
+    <row r="145" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C145" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C125" t="s">
+    <row r="146" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C146" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C126" t="s">
+    <row r="147" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C147" t="s">
         <v>134</v>
       </c>
     </row>
@@ -1785,4 +2134,145 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:C29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>25.1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="27" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="29" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>151</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>